<commit_message>
au cafe et au tabac
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewlekhacman/go/src/github.com/lekhacman/french/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF401EC-FF26-D548-A6BB-968E20419C53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E0278B-63F0-CC4D-93FE-9C381054960F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15200" yWindow="-20720" windowWidth="24060" windowHeight="17540" xr2:uid="{D8ED466C-B49E-5F46-9F15-EBAB31A0E30C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="817">
   <si>
     <t>English</t>
   </si>
@@ -2396,6 +2396,114 @@
   </si>
   <si>
     <t>hurry up (you)</t>
+  </si>
+  <si>
+    <t>quatrième leçon</t>
+  </si>
+  <si>
+    <t>ka.tʁi.jɛm</t>
+  </si>
+  <si>
+    <t>commandons</t>
+  </si>
+  <si>
+    <t>kɔ.mɑ̃.do</t>
+  </si>
+  <si>
+    <t>noirs</t>
+  </si>
+  <si>
+    <t>let's order</t>
+  </si>
+  <si>
+    <t>bơ</t>
+  </si>
+  <si>
+    <t>nwaʁ</t>
+  </si>
+  <si>
+    <t>bières</t>
+  </si>
+  <si>
+    <t>verre</t>
+  </si>
+  <si>
+    <t>blanc</t>
+  </si>
+  <si>
+    <t>bjɛʁ</t>
+  </si>
+  <si>
+    <t>al.mɑ̃</t>
+  </si>
+  <si>
+    <t>vɛʁ</t>
+  </si>
+  <si>
+    <t>blɑ̃</t>
+  </si>
+  <si>
+    <t>slices (of bread)</t>
+  </si>
+  <si>
+    <t>german</t>
+  </si>
+  <si>
+    <t>allemand / allemandes</t>
+  </si>
+  <si>
+    <t>paquets</t>
+  </si>
+  <si>
+    <t>cigarettes brunes</t>
+  </si>
+  <si>
+    <t>tabac</t>
+  </si>
+  <si>
+    <t>tobacco shop</t>
+  </si>
+  <si>
+    <t>packet</t>
+  </si>
+  <si>
+    <t>brown cigarettes</t>
+  </si>
+  <si>
+    <t>cigare hollandais</t>
+  </si>
+  <si>
+    <t>dutch cigar</t>
+  </si>
+  <si>
+    <t>briquet rouge</t>
+  </si>
+  <si>
+    <t>red lighter</t>
+  </si>
+  <si>
+    <t>je suis désolé</t>
+  </si>
+  <si>
+    <t>im sorry</t>
+  </si>
+  <si>
+    <t>pa.kɛ</t>
+  </si>
+  <si>
+    <t>si.ga.ʁɛt bʁyn</t>
+  </si>
+  <si>
+    <t>si.ga ɔ.lɑ̃.dɛ</t>
+  </si>
+  <si>
+    <t>bʁi.kɛt ʁuʒ</t>
+  </si>
+  <si>
+    <t>ʒə sɥi de.zɔ.le</t>
+  </si>
+  <si>
+    <t>ta.ba</t>
   </si>
 </sst>
 </file>
@@ -2770,11 +2878,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E3DDF3-5F2F-F747-8260-C0F186C497B3}">
-  <dimension ref="A1:E678"/>
+  <dimension ref="A1:E691"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A661" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B678" sqref="B678"/>
+      <pane ySplit="1" topLeftCell="A680" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D697" sqref="D697"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26"/>
@@ -8448,6 +8556,9 @@
       </c>
     </row>
     <row r="674" spans="2:5">
+      <c r="B674" s="3" t="s">
+        <v>796</v>
+      </c>
       <c r="C674" s="3" t="s">
         <v>769</v>
       </c>
@@ -8459,6 +8570,9 @@
       </c>
     </row>
     <row r="675" spans="2:5">
+      <c r="B675" s="3" t="s">
+        <v>787</v>
+      </c>
       <c r="C675" s="3" t="s">
         <v>771</v>
       </c>
@@ -8494,6 +8608,152 @@
       </c>
       <c r="D678" s="3" t="s">
         <v>778</v>
+      </c>
+    </row>
+    <row r="679" spans="2:5">
+      <c r="C679" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="D679" s="3" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="680" spans="2:5">
+      <c r="B680" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="C680" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="D680" s="3" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="681" spans="2:5">
+      <c r="B681" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C681" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="D681" s="3" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="682" spans="2:5">
+      <c r="B682" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C682" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="D682" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="E682" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="683" spans="2:5">
+      <c r="B683" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="C683" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="D683" s="3" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="684" spans="2:5">
+      <c r="B684" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C684" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="D684" s="3" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="685" spans="2:5">
+      <c r="B685" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="C685" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="D685" s="3" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="686" spans="2:5">
+      <c r="B686" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="C686" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="D686" s="3" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="687" spans="2:5">
+      <c r="B687" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="C687" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="D687" s="3" t="s">
+        <v>812</v>
+      </c>
+      <c r="E687" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="688" spans="2:5">
+      <c r="B688" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="C688" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="D688" s="3" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="689" spans="2:4">
+      <c r="B689" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="C689" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="D689" s="3" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="690" spans="2:4">
+      <c r="B690" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="C690" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="D690" s="3" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="691" spans="2:4">
+      <c r="B691" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="C691" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="D691" s="3" t="s">
+        <v>815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
quatrixieme lecon - dans la rue
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewlekhacman/go/src/github.com/lekhacman/french/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E0278B-63F0-CC4D-93FE-9C381054960F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D90F05E-80F7-B94D-B883-3CAE394285A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15200" yWindow="-20720" windowWidth="24060" windowHeight="17540" xr2:uid="{D8ED466C-B49E-5F46-9F15-EBAB31A0E30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="878">
   <si>
     <t>English</t>
   </si>
@@ -2504,6 +2505,189 @@
   </si>
   <si>
     <t>ta.ba</t>
+  </si>
+  <si>
+    <t>dans</t>
+  </si>
+  <si>
+    <t>la rue</t>
+  </si>
+  <si>
+    <t>dɑ̃</t>
+  </si>
+  <si>
+    <t>la ʁy</t>
+  </si>
+  <si>
+    <t>du</t>
+  </si>
+  <si>
+    <t>feu</t>
+  </si>
+  <si>
+    <t>fume</t>
+  </si>
+  <si>
+    <t>plus</t>
+  </si>
+  <si>
+    <t>dy</t>
+  </si>
+  <si>
+    <t>fø</t>
+  </si>
+  <si>
+    <t>ply</t>
+  </si>
+  <si>
+    <t>fym</t>
+  </si>
+  <si>
+    <t>the road</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
+  <si>
+    <t>fire</t>
+  </si>
+  <si>
+    <t>smoke</t>
+  </si>
+  <si>
+    <t>plus/more</t>
+  </si>
+  <si>
+    <t>route</t>
+  </si>
+  <si>
+    <t>la table</t>
+  </si>
+  <si>
+    <t>la route</t>
+  </si>
+  <si>
+    <t>l'arbre</t>
+  </si>
+  <si>
+    <t>tabl</t>
+  </si>
+  <si>
+    <t>ʁut</t>
+  </si>
+  <si>
+    <t>aʁbʁ</t>
+  </si>
+  <si>
+    <t>un</t>
+  </si>
+  <si>
+    <t>deux</t>
+  </si>
+  <si>
+    <t>trois</t>
+  </si>
+  <si>
+    <t>quatre</t>
+  </si>
+  <si>
+    <t>cinq</t>
+  </si>
+  <si>
+    <t>sept</t>
+  </si>
+  <si>
+    <t>huit</t>
+  </si>
+  <si>
+    <t>neuf</t>
+  </si>
+  <si>
+    <t>dix</t>
+  </si>
+  <si>
+    <t>onze</t>
+  </si>
+  <si>
+    <t>douze</t>
+  </si>
+  <si>
+    <t>treize</t>
+  </si>
+  <si>
+    <t>quatorze</t>
+  </si>
+  <si>
+    <t>quinze</t>
+  </si>
+  <si>
+    <t>seize</t>
+  </si>
+  <si>
+    <t>dix-sept</t>
+  </si>
+  <si>
+    <t>dix-huit</t>
+  </si>
+  <si>
+    <t>dix-neuf</t>
+  </si>
+  <si>
+    <t>vignt</t>
+  </si>
+  <si>
+    <t>œ̃ / ɛ̃</t>
+  </si>
+  <si>
+    <t>dø</t>
+  </si>
+  <si>
+    <t>tʁwɑ</t>
+  </si>
+  <si>
+    <t>katʁ</t>
+  </si>
+  <si>
+    <t>sɛ̃k</t>
+  </si>
+  <si>
+    <t>sis</t>
+  </si>
+  <si>
+    <t>sɛt</t>
+  </si>
+  <si>
+    <t>ɥit</t>
+  </si>
+  <si>
+    <t>nœf</t>
+  </si>
+  <si>
+    <t>dis</t>
+  </si>
+  <si>
+    <t>ɔ̃z</t>
+  </si>
+  <si>
+    <t>duz</t>
+  </si>
+  <si>
+    <t>tʁɛz</t>
+  </si>
+  <si>
+    <t>ka.tɔʁz</t>
+  </si>
+  <si>
+    <t>kɛ̃z</t>
+  </si>
+  <si>
+    <t>sɛz</t>
+  </si>
+  <si>
+    <t>vɛ̃</t>
+  </si>
+  <si>
+    <t>di.zɥit</t>
   </si>
 </sst>
 </file>
@@ -2878,11 +3062,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E3DDF3-5F2F-F747-8260-C0F186C497B3}">
-  <dimension ref="A1:E691"/>
+  <dimension ref="A1:E721"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A680" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D697" sqref="D697"/>
+      <pane ySplit="1" topLeftCell="A707" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D719" sqref="D719"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26"/>
@@ -8723,7 +8907,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="689" spans="2:4">
+    <row r="689" spans="2:5">
       <c r="B689" s="3" t="s">
         <v>806</v>
       </c>
@@ -8734,7 +8918,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="690" spans="2:4">
+    <row r="690" spans="2:5">
       <c r="B690" s="3" t="s">
         <v>808</v>
       </c>
@@ -8745,7 +8929,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="691" spans="2:4">
+    <row r="691" spans="2:5">
       <c r="B691" s="3" t="s">
         <v>810</v>
       </c>
@@ -8754,6 +8938,342 @@
       </c>
       <c r="D691" s="3" t="s">
         <v>815</v>
+      </c>
+    </row>
+    <row r="692" spans="2:5">
+      <c r="B692" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C692" s="3" t="s">
+        <v>817</v>
+      </c>
+      <c r="D692" s="3" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="693" spans="2:5">
+      <c r="B693" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="C693" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="D693" s="3" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="694" spans="2:5">
+      <c r="B694" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="C694" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="D694" s="3" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="695" spans="2:5">
+      <c r="B695" s="3" t="s">
+        <v>831</v>
+      </c>
+      <c r="C695" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="D695" s="3" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="696" spans="2:5">
+      <c r="B696" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="C696" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="D696" s="3" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="697" spans="2:5">
+      <c r="B697" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="C697" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="D697" s="3" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="698" spans="2:5">
+      <c r="B698" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="C698" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="D698" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="E698" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="699" spans="2:5">
+      <c r="B699" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="C699" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="D699" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="E699" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="700" spans="2:5">
+      <c r="B700" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="C700" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="D700" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="E700" s="3" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="701" spans="2:5">
+      <c r="B701" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="C701" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="D701" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="E701" s="3" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="702" spans="2:5">
+      <c r="B702" s="1">
+        <v>1</v>
+      </c>
+      <c r="C702" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="D702" s="3" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="703" spans="2:5">
+      <c r="B703" s="1">
+        <v>2</v>
+      </c>
+      <c r="C703" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="D703" s="3" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="704" spans="2:5">
+      <c r="B704" s="1">
+        <v>3</v>
+      </c>
+      <c r="C704" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="D704" s="3" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="705" spans="2:4">
+      <c r="B705" s="1">
+        <v>4</v>
+      </c>
+      <c r="C705" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="D705" s="3" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="706" spans="2:4">
+      <c r="B706" s="1">
+        <v>5</v>
+      </c>
+      <c r="C706" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="D706" s="3" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="707" spans="2:4">
+      <c r="B707" s="1">
+        <v>6</v>
+      </c>
+      <c r="C707" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="D707" s="3" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="708" spans="2:4">
+      <c r="B708" s="1">
+        <v>7</v>
+      </c>
+      <c r="C708" s="3" t="s">
+        <v>846</v>
+      </c>
+      <c r="D708" s="3" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="709" spans="2:4">
+      <c r="B709" s="1">
+        <v>8</v>
+      </c>
+      <c r="C709" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="D709" s="3" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="710" spans="2:4">
+      <c r="B710" s="1">
+        <v>9</v>
+      </c>
+      <c r="C710" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="D710" s="3" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="711" spans="2:4">
+      <c r="B711" s="1">
+        <v>10</v>
+      </c>
+      <c r="C711" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="D711" s="3" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="712" spans="2:4">
+      <c r="B712" s="1">
+        <v>11</v>
+      </c>
+      <c r="C712" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="D712" s="3" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="713" spans="2:4">
+      <c r="B713" s="1">
+        <v>12</v>
+      </c>
+      <c r="C713" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="D713" s="3" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="714" spans="2:4">
+      <c r="B714" s="1">
+        <v>13</v>
+      </c>
+      <c r="C714" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="D714" s="3" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="715" spans="2:4">
+      <c r="B715" s="1">
+        <v>14</v>
+      </c>
+      <c r="C715" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="D715" s="3" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="716" spans="2:4">
+      <c r="B716" s="1">
+        <v>15</v>
+      </c>
+      <c r="C716" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="D716" s="3" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="717" spans="2:4">
+      <c r="B717" s="1">
+        <v>16</v>
+      </c>
+      <c r="C717" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="D717" s="3" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="718" spans="2:4">
+      <c r="B718" s="1">
+        <v>17</v>
+      </c>
+      <c r="C718" s="3" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="719" spans="2:4">
+      <c r="B719" s="1">
+        <v>18</v>
+      </c>
+      <c r="C719" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="D719" s="3" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="720" spans="2:4">
+      <c r="B720" s="1">
+        <v>19</v>
+      </c>
+      <c r="C720" s="3" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="721" spans="2:4">
+      <c r="B721" s="1">
+        <v>20</v>
+      </c>
+      <c r="C721" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="D721" s="3" t="s">
+        <v>876</v>
       </c>
     </row>
   </sheetData>
@@ -8761,4 +9281,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA89DD5-CD61-8B46-9219-77CA9EA380CB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="26"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>